<commit_message>
Created dataframe for algorithm
</commit_message>
<xml_diff>
--- a/DataVisualizationV5.xlsx
+++ b/DataVisualizationV5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chakotay Incorvaia\dev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598549A-2086-4729-90E5-EA382CBACBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A08FDD6-2ED3-4795-803E-0E885C95A2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Reliable</t>
   </si>
   <si>
-    <t>Redundany</t>
-  </si>
-  <si>
     <t>Trainability and Learnability</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>5,12</t>
+  </si>
+  <si>
+    <t>Redundancy</t>
   </si>
 </sst>
 </file>
@@ -576,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A2CE25-1FB0-46F3-A95B-A7BCC2B1E34D}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B39" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,49 +611,49 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3">
         <v>5</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="3">
         <v>4</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>3</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3">
         <v>5</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="3">
         <v>4</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="3">
         <v>4</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
@@ -2011,17 +2011,6 @@
       <c r="O27" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2053,54 +2042,54 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2147,7 +2136,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2194,7 +2183,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2241,7 +2230,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2288,7 +2277,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2335,7 +2324,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2382,7 +2371,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2429,7 +2418,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2476,7 +2465,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2523,7 +2512,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2570,7 +2559,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2617,7 +2606,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2664,7 +2653,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2711,7 +2700,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2785,54 +2774,54 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2879,7 +2868,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2926,7 +2915,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2959,7 +2948,7 @@
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4">
         <v>7</v>
@@ -2973,7 +2962,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3020,7 +3009,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3067,7 +3056,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3114,7 +3103,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3161,7 +3150,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3208,7 +3197,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3255,7 +3244,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3302,7 +3291,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3349,7 +3338,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3396,7 +3385,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3443,7 +3432,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3517,54 +3506,54 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3611,7 +3600,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3658,7 +3647,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3691,7 +3680,7 @@
         <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4">
         <v>11</v>
@@ -3705,7 +3694,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>17</v>
@@ -3752,7 +3741,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3799,7 +3788,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3846,7 +3835,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3893,7 +3882,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>28</v>
@@ -3940,7 +3929,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3987,7 +3976,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4034,7 +4023,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4081,7 +4070,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4128,7 +4117,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4175,7 +4164,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4240,18 +4229,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>230</v>
@@ -4262,7 +4251,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>210</v>
@@ -4273,7 +4262,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -4284,7 +4273,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>152</v>
@@ -4295,7 +4284,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>228</v>
@@ -4306,7 +4295,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>152</v>
@@ -4317,7 +4306,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>171</v>
@@ -4328,7 +4317,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>114</v>
@@ -4339,7 +4328,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>67</v>
@@ -4350,7 +4339,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>67</v>
@@ -4361,7 +4350,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>210</v>
@@ -4372,7 +4361,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>64</v>
@@ -4383,7 +4372,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>228</v>
@@ -4394,7 +4383,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>210</v>

</xml_diff>

<commit_message>
WIP graphs created - not yet with weights
</commit_message>
<xml_diff>
--- a/DataVisualizationV5.xlsx
+++ b/DataVisualizationV5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6232E89-EF5D-4BF1-919E-C4034E4341BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73106550-6BBC-4714-B679-7D3D53BD14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
@@ -2022,7 +2022,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="A1:XFD1048576"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,7 +2753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25054DBB-0C9E-4774-836A-94537D3FE0A1}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -3485,8 +3485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F027EA97-39C6-4A00-847A-7E78910072DF}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C56" sqref="C55:C56"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Graph includes all nodes
</commit_message>
<xml_diff>
--- a/DataVisualizationV5.xlsx
+++ b/DataVisualizationV5.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73106550-6BBC-4714-B679-7D3D53BD14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D515DB9-99DD-4C82-9F87-0FC317C4EE40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="1395" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
     <sheet name="PhaseSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="PhaseSheet2" sheetId="6" r:id="rId3"/>
-    <sheet name="SequenceSheet" sheetId="3" r:id="rId4"/>
-    <sheet name="EntireSequenceSheet" sheetId="4" r:id="rId5"/>
-    <sheet name="SizeSpec" sheetId="5" r:id="rId6"/>
+    <sheet name="SequenceSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="EntireSequenceSheet" sheetId="4" r:id="rId4"/>
+    <sheet name="SizeSpec" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="61">
   <si>
     <t>Accuracy</t>
   </si>
@@ -577,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A2CE25-1FB0-46F3-A95B-A7BCC2B1E34D}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B39" sqref="B38:B39"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,7 +2021,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,11 +2749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25054DBB-0C9E-4774-836A-94537D3FE0A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F027EA97-39C6-4A00-847A-7E78910072DF}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,13 +2828,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2923,40 +2922,40 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3000,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -3070,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3094,10 +3093,10 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3132,10 +3131,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -3144,7 +3143,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3152,7 +3151,7 @@
         <v>48</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3179,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -3205,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3235,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -3249,10 +3248,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3261,16 +3260,16 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3296,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3379,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3461,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -3482,11 +3481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F027EA97-39C6-4A00-847A-7E78910072DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EC5F28-856E-4AB6-A730-1C22BA4C9B5A}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3602,7 +3601,7 @@
         <v>42</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -3655,40 +3654,40 @@
         <v>0</v>
       </c>
       <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
+      </c>
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4">
-        <v>7</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
       <c r="O4">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3696,7 +3695,7 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3732,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -3799,10 +3798,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3826,10 +3825,10 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="O7">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3846,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -3864,10 +3863,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -3876,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3884,10 +3883,10 @@
         <v>48</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3911,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -3934,10 +3933,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3967,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -3981,10 +3980,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3993,16 +3992,16 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -4014,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -4028,10 +4027,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -4075,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4111,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4193,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -4205,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4214,738 +4213,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EC5F28-856E-4AB6-A730-1C22BA4C9B5A}">
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>14</v>
-      </c>
-      <c r="K4">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4">
-        <v>11</v>
-      </c>
-      <c r="N4">
-        <v>6</v>
-      </c>
-      <c r="O4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>18</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>22</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>20</v>
-      </c>
-      <c r="O7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>23</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>26</v>
-      </c>
-      <c r="L8">
-        <v>25</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9">
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>29</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>32</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>34</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>36</v>
-      </c>
-      <c r="H11">
-        <v>37</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>38</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>33</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>39</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>41</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>44</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C30AA8-3415-4BDB-A606-A9FA09E8CC8D}">
   <dimension ref="A1:C15"/>
   <sheetViews>

</xml_diff>

<commit_message>
WIP adding node weights
</commit_message>
<xml_diff>
--- a/DataVisualizationV5.xlsx
+++ b/DataVisualizationV5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D515DB9-99DD-4C82-9F87-0FC317C4EE40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCB4B1-8321-44B1-B475-CD932B8E7824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>